<commit_message>
Added data labels to the chart
</commit_message>
<xml_diff>
--- a/report_2021.xlsx
+++ b/report_2021.xlsx
@@ -303,6 +303,9 @@
             </numRef>
           </val>
         </ser>
+        <dLbls>
+          <showVal val="1"/>
+        </dLbls>
         <gapWidth val="150"/>
         <axId val="10"/>
         <axId val="100"/>
@@ -348,7 +351,7 @@
       <row>11</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7200000" cy="5400000"/>
+    <ext cx="9000000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>

</xml_diff>